<commit_message>
update varius - add sql connect in Room - add method about problem - add attribute for check in Problem - edit problemname
</commit_message>
<xml_diff>
--- a/ListProblem.xlsx
+++ b/ListProblem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -35,9 +35,6 @@
     <t>กระจกแตก</t>
   </si>
   <si>
-    <t>กรประตูเสีย</t>
-  </si>
-  <si>
     <t>ฟักบัวเสีย</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>ตู้เสื้อผ้าเจ้ง</t>
+  </si>
+  <si>
+    <t>ประตูเสีย</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -511,13 +511,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -525,13 +525,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -539,13 +539,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -553,13 +553,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -567,13 +567,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -581,13 +581,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -595,13 +595,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -609,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -617,7 +617,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -625,7 +625,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -633,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -641,7 +641,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -649,7 +649,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -657,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -665,7 +665,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -673,7 +673,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -681,7 +681,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -689,7 +689,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>